<commit_message>
Lets keep this going
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AB3458-751B-4178-B55A-142445EA82D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBFB752-92D5-4C54-9AD5-DCDA033F119E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>url</t>
   </si>
@@ -67,6 +67,27 @@
   </si>
   <si>
     <t>utilize a sliding window approach with a dictionary to track character indices.</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>utilize a two-pointer approach with a sliding window technique.</t>
+  </si>
+  <si>
+    <t>Container With Most Water</t>
+  </si>
+  <si>
+    <t>Longest Substring Without Repeating Characters</t>
+  </si>
+  <si>
+    <t>Two Sum</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>http://rb.gy/oual6</t>
   </si>
 </sst>
 </file>
@@ -407,85 +428,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F4"/>
+  <dimension ref="A2:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="18.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="47.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="84.5546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="https://leetcode.com/problems/two-sum/description/" xr:uid="{D29A1F65-8394-4D89-BD96-17CD60D15AFD}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{3A7CEF42-3337-4C95-84AC-B7CAF9B28B7F}"/>
+    <hyperlink ref="D3" r:id="rId1" display="https://leetcode.com/problems/two-sum/description/" xr:uid="{D29A1F65-8394-4D89-BD96-17CD60D15AFD}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{3A7CEF42-3337-4C95-84AC-B7CAF9B28B7F}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{6B70FD5E-C0D2-445D-BDB3-4DB279AB8A7B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Solved and easy leetcode
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\OneDrive - ARK\programs\code\leetcode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://agnesh-my.sharepoint.com/personal/agnesh_agnesh_onmicrosoft_com/Documents/programs/code/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF1F131-368A-43AB-859E-D934125EBA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{DAF1F131-368A-43AB-859E-D934125EBA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47D8D20A-3D07-4C0D-AD2E-F3808825D3FE}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4185" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>url</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t xml:space="preserve">Use pointers </t>
+  </si>
+  <si>
+    <t>Middle of the Linked List</t>
+  </si>
+  <si>
+    <t>http://rb.gy/nrugfa</t>
+  </si>
+  <si>
+    <t>Use a slow and a fast pointer.</t>
   </si>
 </sst>
 </file>
@@ -476,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,6 +683,29 @@
         <v>36</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>876</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G8">
     <sortCondition ref="A2:A8"/>
@@ -686,6 +718,7 @@
     <hyperlink ref="D5" r:id="rId5" xr:uid="{68AE57ED-F523-4FD0-8423-21CCC6C328A5}"/>
     <hyperlink ref="D6" r:id="rId6" xr:uid="{7E99A919-0A12-4725-AEEE-0A6D4B0AEBE8}"/>
     <hyperlink ref="D8" r:id="rId7" xr:uid="{2E4AB602-75C1-45E8-B9E9-1B16196F8BB9}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{9FDD29CA-7B6F-4D9C-B8AB-2CA22F1BD75D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2 sum 2 done
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agneshk\pc\data\leetcode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\OneDrive - ARK\programs\code\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFBFD26-3A76-46F0-8225-DB8E3AB35DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F7020D-8122-448D-AD64-1468E7835E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
   <si>
     <t>url</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>Use slow and fast pointer.</t>
+  </si>
+  <si>
+    <t>Two Sum II - Input Array Is Sorted</t>
+  </si>
+  <si>
+    <t>http://rb.gy/psjwn9</t>
+  </si>
+  <si>
+    <t>Use left and right pointers and the fact that the array is sorted</t>
   </si>
 </sst>
 </file>
@@ -515,24 +524,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.88671875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="84.5546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="84.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -555,7 +564,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -578,7 +587,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -601,7 +610,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>11</v>
       </c>
@@ -624,7 +633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>19</v>
       </c>
@@ -647,7 +656,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>46</v>
       </c>
@@ -667,7 +676,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>94</v>
       </c>
@@ -690,7 +699,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>104</v>
       </c>
@@ -713,7 +722,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>147</v>
       </c>
@@ -736,78 +745,101 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
+        <v>167</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>206</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>234</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>876</v>
+        <v>234</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>876</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="F13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
-    <sortCondition ref="A1:A12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G13">
+    <sortCondition ref="A2:A13"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://leetcode.com/problems/two-sum/description/" xr:uid="{D29A1F65-8394-4D89-BD96-17CD60D15AFD}"/>
@@ -816,11 +848,12 @@
     <hyperlink ref="D9" r:id="rId4" xr:uid="{A248292A-243F-409F-94AA-C731025CF02A}"/>
     <hyperlink ref="D6" r:id="rId5" xr:uid="{68AE57ED-F523-4FD0-8423-21CCC6C328A5}"/>
     <hyperlink ref="D7" r:id="rId6" xr:uid="{7E99A919-0A12-4725-AEEE-0A6D4B0AEBE8}"/>
-    <hyperlink ref="D10" r:id="rId7" xr:uid="{2E4AB602-75C1-45E8-B9E9-1B16196F8BB9}"/>
-    <hyperlink ref="D12" r:id="rId8" xr:uid="{9FDD29CA-7B6F-4D9C-B8AB-2CA22F1BD75D}"/>
+    <hyperlink ref="D11" r:id="rId7" xr:uid="{2E4AB602-75C1-45E8-B9E9-1B16196F8BB9}"/>
+    <hyperlink ref="D13" r:id="rId8" xr:uid="{9FDD29CA-7B6F-4D9C-B8AB-2CA22F1BD75D}"/>
     <hyperlink ref="D8" r:id="rId9" xr:uid="{D47E6F13-2C77-4D9C-A0C2-3A61BB7DB7F7}"/>
-    <hyperlink ref="D11" r:id="rId10" xr:uid="{9C7F51E0-A421-48E3-A675-090808C1F22C}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{9C7F51E0-A421-48E3-A675-090808C1F22C}"/>
     <hyperlink ref="D5" r:id="rId11" xr:uid="{E51C5646-FEE1-44F7-91C4-364A6DFCFF85}"/>
+    <hyperlink ref="D10" r:id="rId12" xr:uid="{D3E7F543-6809-4756-9AED-0E4868030A9A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes in two sum 2
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agneshk\pc\code\leetcode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agneshk\pc\data\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF68DD9-A4BF-4723-A874-7ABC85A538E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA411C4-B31D-47F8-86D3-81F74FF23A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t>url</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>https://rebrand.ly/e3bo9ay</t>
-  </si>
-  <si>
-    <t>O(log(n))</t>
   </si>
   <si>
     <t>Use Binary Search Algorithm along with two pointer technique.</t>
@@ -584,7 +581,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -812,7 +809,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>53</v>
@@ -821,10 +818,10 @@
         <v>35</v>
       </c>
       <c r="F10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added about 3 sum
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agneshk\pc\data\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA411C4-B31D-47F8-86D3-81F74FF23A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B0C03E-69CA-441A-BD49-CA4E127133BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -581,7 +581,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added merge two sorted lists
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agneshk\pc\data\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D04218-BC65-4817-BC80-B22CDD276318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43498D07-F08D-4DD4-BBDE-788A012443B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
   <si>
     <t>url</t>
   </si>
@@ -202,6 +202,15 @@
   </si>
   <si>
     <t>Use a stack</t>
+  </si>
+  <si>
+    <t>https://rebrand.ly/4t4p9zb</t>
+  </si>
+  <si>
+    <t>Use two pointers on each list and keep comparing until one goes invalid. Append the remaining to the result.</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Lists</t>
   </si>
 </sst>
 </file>
@@ -587,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,7 +610,7 @@
     <col min="4" max="4" width="24.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="84.5546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="101.77734375" style="3" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
@@ -946,6 +955,29 @@
       </c>
       <c r="G15" s="6" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>21</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -967,8 +999,9 @@
     <hyperlink ref="D12" r:id="rId12" xr:uid="{EA1E0AA8-8F6F-4265-84F0-6C4AB0FA52AB}"/>
     <hyperlink ref="D10" r:id="rId13" xr:uid="{1D16F9F4-D9DC-49D7-A64B-F7F293ADC1B4}"/>
     <hyperlink ref="D15" r:id="rId14" xr:uid="{8550C157-C895-4E10-8151-A29957550A7F}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{2BC18D0F-9C3B-484A-9BAB-F5F1860DAAB1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reverse substring between each pair of parentheses
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\OneDrive - ARK\programs\code\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C8264E-E17D-443E-AA4C-34BEA62B69C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CF3D5F-E39B-46E1-937C-E78608CC18C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
   <si>
     <t>url</t>
   </si>
@@ -220,6 +220,15 @@
   </si>
   <si>
     <t>Solve by drawing a timeline</t>
+  </si>
+  <si>
+    <t>Reverse Substrings Between Each Pair of Parentheses</t>
+  </si>
+  <si>
+    <t>http://rb.gy/0h2e8g</t>
+  </si>
+  <si>
+    <t>Use the stack cleverly</t>
   </si>
 </sst>
 </file>
@@ -605,17 +614,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="51.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
@@ -715,7 +724,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>19</v>
       </c>
@@ -1008,6 +1017,29 @@
       </c>
       <c r="G17" s="9" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>1190</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1031,8 +1063,9 @@
     <hyperlink ref="D15" r:id="rId14" xr:uid="{8550C157-C895-4E10-8151-A29957550A7F}"/>
     <hyperlink ref="D16" r:id="rId15" xr:uid="{2BC18D0F-9C3B-484A-9BAB-F5F1860DAAB1}"/>
     <hyperlink ref="D17" r:id="rId16" xr:uid="{3651F195-4484-4B60-9381-160A18299D79}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{636A9039-9CA1-4DCC-A5DB-79562BBBC056}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the solution notes for max depth of binary tree
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agneshk\pc\data\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CCA355-5E11-45D5-B351-76310804F460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674A4111-5902-408C-8F95-593B96B3094F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>difficulty</t>
   </si>
   <si>
-    <t>datastructure</t>
-  </si>
-  <si>
     <t>efficient O</t>
   </si>
   <si>
@@ -241,6 +238,9 @@
   </si>
   <si>
     <t>Use recurrsion cleverly</t>
+  </si>
+  <si>
+    <t>Approach</t>
   </si>
 </sst>
 </file>
@@ -312,7 +312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -345,6 +345,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -626,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,19 +655,19 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="4" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -672,22 +675,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -695,22 +698,22 @@
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -718,22 +721,22 @@
         <v>11</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -741,22 +744,22 @@
         <v>19</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -764,20 +767,20 @@
         <v>46</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>26</v>
-      </c>
       <c r="E6" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -785,22 +788,22 @@
         <v>94</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -808,22 +811,22 @@
         <v>104</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -831,22 +834,22 @@
         <v>147</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>17</v>
-      </c>
       <c r="F9" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -854,22 +857,22 @@
         <v>167</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -877,22 +880,22 @@
         <v>206</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -900,22 +903,22 @@
         <v>230</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -923,22 +926,22 @@
         <v>234</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -946,22 +949,22 @@
         <v>876</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -969,22 +972,22 @@
         <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -992,22 +995,22 @@
         <v>21</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1015,20 +1018,20 @@
         <v>1701</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>63</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1036,22 +1039,22 @@
         <v>1190</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="E18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1059,23 +1062,26 @@
         <v>100</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="F19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>71</v>
-      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D20" s="12"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G14">

</xml_diff>

<commit_message>
solved invert binary tree
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agneshk\pc\data\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674A4111-5902-408C-8F95-593B96B3094F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A003D1CE-5E46-4998-836F-4BD9ED6F93CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
   <si>
     <t>url</t>
   </si>
@@ -241,6 +241,15 @@
   </si>
   <si>
     <t>Approach</t>
+  </si>
+  <si>
+    <t>Invert Binary Tree</t>
+  </si>
+  <si>
+    <t>https://shorturl.at/Lq38f</t>
+  </si>
+  <si>
+    <t>Simple recursion</t>
   </si>
 </sst>
 </file>
@@ -312,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -345,9 +354,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -632,7 +638,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1081,7 +1087,27 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D20" s="12"/>
+      <c r="A20" s="5">
+        <v>226</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G14">
@@ -1106,8 +1132,9 @@
     <hyperlink ref="D17" r:id="rId16" xr:uid="{3651F195-4484-4B60-9381-160A18299D79}"/>
     <hyperlink ref="D18" r:id="rId17" xr:uid="{636A9039-9CA1-4DCC-A5DB-79562BBBC056}"/>
     <hyperlink ref="D19" r:id="rId18" xr:uid="{DC17FDF3-9A9B-4FEA-9D6A-DF4252E08036}"/>
+    <hyperlink ref="D20" r:id="rId19" xr:uid="{6F6969B7-A411-4085-9E8F-58E3BF1FF942}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
solved binary tree level order traversal
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agneshk\pc\data\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A003D1CE-5E46-4998-836F-4BD9ED6F93CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D0700E-E50D-4512-B674-CBB9E5A0E35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="79">
   <si>
     <t>url</t>
   </si>
@@ -250,6 +250,18 @@
   </si>
   <si>
     <t>Simple recursion</t>
+  </si>
+  <si>
+    <t>Binary Tree Level Order Traversal</t>
+  </si>
+  <si>
+    <t>https://shorturl.at/89NnQ</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>Use DFS using queues and use a counter variable (size) to get the level arrays inside the res array.</t>
   </si>
 </sst>
 </file>
@@ -635,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1107,6 +1119,29 @@
       </c>
       <c r="G20" s="6" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>102</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1133,8 +1168,9 @@
     <hyperlink ref="D18" r:id="rId17" xr:uid="{636A9039-9CA1-4DCC-A5DB-79562BBBC056}"/>
     <hyperlink ref="D19" r:id="rId18" xr:uid="{DC17FDF3-9A9B-4FEA-9D6A-DF4252E08036}"/>
     <hyperlink ref="D20" r:id="rId19" xr:uid="{6F6969B7-A411-4085-9E8F-58E3BF1FF942}"/>
+    <hyperlink ref="D21" r:id="rId20" xr:uid="{CA194911-BED7-40B0-B5B4-D5638F409E73}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Brute forced subtree of another tree
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agneshk\pc\data\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D0700E-E50D-4512-B674-CBB9E5A0E35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71787E5-6282-46FB-BE2E-352404FFABE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="85">
   <si>
     <t>url</t>
   </si>
@@ -262,12 +262,33 @@
   </si>
   <si>
     <t>Use DFS using queues and use a counter variable (size) to get the level arrays inside the res array.</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Subtree of Another Tree</t>
+  </si>
+  <si>
+    <t>https://shorturl.at/MWP2V</t>
+  </si>
+  <si>
+    <t>BFS + Recursion</t>
+  </si>
+  <si>
+    <t>O(n^2)</t>
+  </si>
+  <si>
+    <t>Use BFS and the algorithm the check is two trees are same (lc 100: same tree)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -333,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -366,6 +387,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -647,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A22" sqref="A22:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,10 +688,11 @@
     <col min="5" max="5" width="13.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="101.6640625" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="11"/>
+    <col min="8" max="8" width="11.21875" style="13" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -687,8 +714,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H1" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -710,8 +740,9 @@
       <c r="G2" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>3</v>
       </c>
@@ -734,7 +765,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>11</v>
       </c>
@@ -757,7 +788,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>19</v>
       </c>
@@ -780,7 +811,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>46</v>
       </c>
@@ -801,7 +832,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>94</v>
       </c>
@@ -824,7 +855,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>104</v>
       </c>
@@ -847,7 +878,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>147</v>
       </c>
@@ -870,7 +901,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>167</v>
       </c>
@@ -893,7 +924,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>206</v>
       </c>
@@ -916,7 +947,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>230</v>
       </c>
@@ -939,7 +970,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>234</v>
       </c>
@@ -962,7 +993,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>876</v>
       </c>
@@ -985,7 +1016,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>20</v>
       </c>
@@ -1008,7 +1039,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>21</v>
       </c>
@@ -1031,7 +1062,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>1701</v>
       </c>
@@ -1052,7 +1083,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>1190</v>
       </c>
@@ -1075,7 +1106,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>100</v>
       </c>
@@ -1098,7 +1129,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>226</v>
       </c>
@@ -1121,7 +1152,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>102</v>
       </c>
@@ -1142,6 +1173,32 @@
       </c>
       <c r="G21" s="6" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>572</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H22" s="14">
+        <v>45492</v>
       </c>
     </row>
   </sheetData>
@@ -1169,8 +1226,9 @@
     <hyperlink ref="D19" r:id="rId18" xr:uid="{DC17FDF3-9A9B-4FEA-9D6A-DF4252E08036}"/>
     <hyperlink ref="D20" r:id="rId19" xr:uid="{6F6969B7-A411-4085-9E8F-58E3BF1FF942}"/>
     <hyperlink ref="D21" r:id="rId20" xr:uid="{CA194911-BED7-40B0-B5B4-D5638F409E73}"/>
+    <hyperlink ref="D22" r:id="rId21" xr:uid="{3BF7A565-83B5-4AAE-BAC3-B58A69DEAE20}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
solved sort the jumbled numbers
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agneshk\pc\data\leetcode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\OneDrive - ARK\programs\code\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7E80E1-8FDC-4130-BF3F-D8F420D8EF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3E0738-3C02-4D82-97D1-8981FFBE3314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="93">
   <si>
     <t>url</t>
   </si>
@@ -289,6 +289,21 @@
   </si>
   <si>
     <t>Non-intuitive logic, but forming the test cases and then testing the solution works</t>
+  </si>
+  <si>
+    <t>Sort the Jumbled Numbers</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sort-the-jumbled-numbers/description/</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>O(nd+logn)</t>
+  </si>
+  <si>
+    <t>Encode the numbers according to the map, store (encoded_num, index) in a list. Exploit python's sort feature. Check the notes, this is good problem.</t>
   </si>
 </sst>
 </file>
@@ -682,26 +697,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="D9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="51.44140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="101.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.21875" style="13" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="11"/>
+    <col min="1" max="1" width="8.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="101.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="13" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -727,7 +742,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -751,7 +766,7 @@
       </c>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>3</v>
       </c>
@@ -774,7 +789,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>11</v>
       </c>
@@ -797,7 +812,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>19</v>
       </c>
@@ -820,7 +835,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>46</v>
       </c>
@@ -841,7 +856,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>94</v>
       </c>
@@ -864,7 +879,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>104</v>
       </c>
@@ -887,7 +902,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>147</v>
       </c>
@@ -910,7 +925,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>167</v>
       </c>
@@ -933,7 +948,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>206</v>
       </c>
@@ -956,7 +971,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>230</v>
       </c>
@@ -979,7 +994,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>234</v>
       </c>
@@ -1002,7 +1017,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>876</v>
       </c>
@@ -1025,7 +1040,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>20</v>
       </c>
@@ -1048,7 +1063,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>21</v>
       </c>
@@ -1071,7 +1086,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>1701</v>
       </c>
@@ -1092,7 +1107,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>1190</v>
       </c>
@@ -1115,7 +1130,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>100</v>
       </c>
@@ -1138,7 +1153,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>226</v>
       </c>
@@ -1161,7 +1176,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>102</v>
       </c>
@@ -1184,7 +1199,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>572</v>
       </c>
@@ -1210,7 +1225,7 @@
         <v>45492</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>121</v>
       </c>
@@ -1232,6 +1247,32 @@
       </c>
       <c r="H23" s="14">
         <v>45496</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>2191</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="14">
+        <v>45497</v>
       </c>
     </row>
   </sheetData>
@@ -1261,8 +1302,9 @@
     <hyperlink ref="D21" r:id="rId20" xr:uid="{CA194911-BED7-40B0-B5B4-D5638F409E73}"/>
     <hyperlink ref="D22" r:id="rId21" xr:uid="{3BF7A565-83B5-4AAE-BAC3-B58A69DEAE20}"/>
     <hyperlink ref="D23" r:id="rId22" xr:uid="{8D63FD65-E0C5-4A54-BDEF-860350E0B7FD}"/>
+    <hyperlink ref="D24" r:id="rId23" xr:uid="{90C58A53-6B5A-4F1A-AF8C-7CD4898E0DE7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solved my first lc hard
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\OneDrive - ARK\programs\code\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3E0738-3C02-4D82-97D1-8981FFBE3314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257D66A1-FAC6-4757-83FF-E32497841243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
   <si>
     <t>url</t>
   </si>
@@ -304,6 +304,27 @@
   </si>
   <si>
     <t>Encode the numbers according to the map, store (encoded_num, index) in a list. Exploit python's sort feature. Check the notes, this is good problem.</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t>Binary Tree Maximum Path Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-maximum-path-sum/description/</t>
+  </si>
+  <si>
+    <t>Checkout neetcodeio and my recorded video.</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>Binary Tree</t>
+  </si>
+  <si>
+    <t>blind75</t>
   </si>
 </sst>
 </file>
@@ -330,7 +351,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,6 +367,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -378,7 +405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -416,6 +443,17 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -697,26 +735,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="51.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="48" style="3" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="101.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="13" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="11"/>
+    <col min="8" max="8" width="12.85546875" style="13" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="11" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -741,8 +780,11 @@
       <c r="H1" s="12" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -766,7 +808,7 @@
       </c>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>3</v>
       </c>
@@ -789,7 +831,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>11</v>
       </c>
@@ -812,7 +854,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>19</v>
       </c>
@@ -835,476 +877,509 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>46</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>20</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>46</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>94</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="6" t="s">
+      <c r="F9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>100</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>102</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>104</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="F12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>147</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>167</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>206</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>230</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>234</v>
+        <v>121</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>44</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="E13" s="6"/>
       <c r="F13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>876</v>
-      </c>
-      <c r="B14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" s="14">
+        <v>45496</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>142</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H14" s="18">
+        <v>45500</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>147</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>167</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>206</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="6" t="s">
+      <c r="C17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>20</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="F17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>226</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="C18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>230</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>21</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>1701</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>1190</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>100</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>70</v>
+      <c r="F19" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>102</v>
+        <v>572</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>78</v>
+        <v>84</v>
+      </c>
+      <c r="H21" s="14">
+        <v>45492</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>572</v>
+        <v>876</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="H22" s="14">
-        <v>45492</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>121</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="H23" s="14">
-        <v>45496</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>1190</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>1701</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
         <v>2191</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C25" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G25" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H24" s="14">
+      <c r="H25" s="14">
         <v>45497</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G14">
-    <sortCondition ref="A2:A14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J25">
+    <sortCondition ref="A2:A25"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://leetcode.com/problems/two-sum/description/" xr:uid="{D29A1F65-8394-4D89-BD96-17CD60D15AFD}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{3A7CEF42-3337-4C95-84AC-B7CAF9B28B7F}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{6B70FD5E-C0D2-445D-BDB3-4DB279AB8A7B}"/>
-    <hyperlink ref="D9" r:id="rId4" xr:uid="{A248292A-243F-409F-94AA-C731025CF02A}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{68AE57ED-F523-4FD0-8423-21CCC6C328A5}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{7E99A919-0A12-4725-AEEE-0A6D4B0AEBE8}"/>
-    <hyperlink ref="D11" r:id="rId7" xr:uid="{2E4AB602-75C1-45E8-B9E9-1B16196F8BB9}"/>
-    <hyperlink ref="D14" r:id="rId8" xr:uid="{9FDD29CA-7B6F-4D9C-B8AB-2CA22F1BD75D}"/>
-    <hyperlink ref="D8" r:id="rId9" xr:uid="{D47E6F13-2C77-4D9C-A0C2-3A61BB7DB7F7}"/>
-    <hyperlink ref="D13" r:id="rId10" xr:uid="{9C7F51E0-A421-48E3-A675-090808C1F22C}"/>
+    <hyperlink ref="D15" r:id="rId4" xr:uid="{A248292A-243F-409F-94AA-C731025CF02A}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{68AE57ED-F523-4FD0-8423-21CCC6C328A5}"/>
+    <hyperlink ref="D9" r:id="rId6" xr:uid="{7E99A919-0A12-4725-AEEE-0A6D4B0AEBE8}"/>
+    <hyperlink ref="D17" r:id="rId7" xr:uid="{2E4AB602-75C1-45E8-B9E9-1B16196F8BB9}"/>
+    <hyperlink ref="D22" r:id="rId8" xr:uid="{9FDD29CA-7B6F-4D9C-B8AB-2CA22F1BD75D}"/>
+    <hyperlink ref="D12" r:id="rId9" xr:uid="{D47E6F13-2C77-4D9C-A0C2-3A61BB7DB7F7}"/>
+    <hyperlink ref="D20" r:id="rId10" xr:uid="{9C7F51E0-A421-48E3-A675-090808C1F22C}"/>
     <hyperlink ref="D5" r:id="rId11" xr:uid="{E51C5646-FEE1-44F7-91C4-364A6DFCFF85}"/>
-    <hyperlink ref="D12" r:id="rId12" xr:uid="{EA1E0AA8-8F6F-4265-84F0-6C4AB0FA52AB}"/>
-    <hyperlink ref="D10" r:id="rId13" xr:uid="{1D16F9F4-D9DC-49D7-A64B-F7F293ADC1B4}"/>
-    <hyperlink ref="D15" r:id="rId14" xr:uid="{8550C157-C895-4E10-8151-A29957550A7F}"/>
-    <hyperlink ref="D16" r:id="rId15" xr:uid="{2BC18D0F-9C3B-484A-9BAB-F5F1860DAAB1}"/>
-    <hyperlink ref="D17" r:id="rId16" xr:uid="{3651F195-4484-4B60-9381-160A18299D79}"/>
-    <hyperlink ref="D18" r:id="rId17" xr:uid="{636A9039-9CA1-4DCC-A5DB-79562BBBC056}"/>
-    <hyperlink ref="D19" r:id="rId18" xr:uid="{DC17FDF3-9A9B-4FEA-9D6A-DF4252E08036}"/>
-    <hyperlink ref="D20" r:id="rId19" xr:uid="{6F6969B7-A411-4085-9E8F-58E3BF1FF942}"/>
-    <hyperlink ref="D21" r:id="rId20" xr:uid="{CA194911-BED7-40B0-B5B4-D5638F409E73}"/>
-    <hyperlink ref="D22" r:id="rId21" xr:uid="{3BF7A565-83B5-4AAE-BAC3-B58A69DEAE20}"/>
-    <hyperlink ref="D23" r:id="rId22" xr:uid="{8D63FD65-E0C5-4A54-BDEF-860350E0B7FD}"/>
-    <hyperlink ref="D24" r:id="rId23" xr:uid="{90C58A53-6B5A-4F1A-AF8C-7CD4898E0DE7}"/>
+    <hyperlink ref="D19" r:id="rId12" xr:uid="{EA1E0AA8-8F6F-4265-84F0-6C4AB0FA52AB}"/>
+    <hyperlink ref="D16" r:id="rId13" xr:uid="{1D16F9F4-D9DC-49D7-A64B-F7F293ADC1B4}"/>
+    <hyperlink ref="D6" r:id="rId14" xr:uid="{8550C157-C895-4E10-8151-A29957550A7F}"/>
+    <hyperlink ref="D7" r:id="rId15" xr:uid="{2BC18D0F-9C3B-484A-9BAB-F5F1860DAAB1}"/>
+    <hyperlink ref="D24" r:id="rId16" xr:uid="{3651F195-4484-4B60-9381-160A18299D79}"/>
+    <hyperlink ref="D23" r:id="rId17" xr:uid="{636A9039-9CA1-4DCC-A5DB-79562BBBC056}"/>
+    <hyperlink ref="D10" r:id="rId18" xr:uid="{DC17FDF3-9A9B-4FEA-9D6A-DF4252E08036}"/>
+    <hyperlink ref="D18" r:id="rId19" xr:uid="{6F6969B7-A411-4085-9E8F-58E3BF1FF942}"/>
+    <hyperlink ref="D11" r:id="rId20" xr:uid="{CA194911-BED7-40B0-B5B4-D5638F409E73}"/>
+    <hyperlink ref="D21" r:id="rId21" xr:uid="{3BF7A565-83B5-4AAE-BAC3-B58A69DEAE20}"/>
+    <hyperlink ref="D13" r:id="rId22" xr:uid="{8D63FD65-E0C5-4A54-BDEF-860350E0B7FD}"/>
+    <hyperlink ref="D25" r:id="rId23" xr:uid="{90C58A53-6B5A-4F1A-AF8C-7CD4898E0DE7}"/>
+    <hyperlink ref="D14" r:id="rId24" xr:uid="{E3888C7C-DDBB-4226-8610-B38F3E7E7E6D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "update in excel"
This reverts commit f91f60ec96be75f413c21d79ae3d72325c2e596d.
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agneshk\pc\code\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD473CE-EA14-4985-A074-C4BC917AD1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF68DD9-A4BF-4723-A874-7ABC85A538E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
   <si>
     <t>url</t>
   </si>
@@ -189,19 +189,13 @@
     <t>https://rebrand.ly/e3bo9ay</t>
   </si>
   <si>
+    <t>O(log(n))</t>
+  </si>
+  <si>
+    <t>Use Binary Search Algorithm along with two pointer technique.</t>
+  </si>
+  <si>
     <t>Two Sum II - Input Array Is Sorted</t>
-  </si>
-  <si>
-    <t>3sum</t>
-  </si>
-  <si>
-    <t>https://rebrand.ly/hvgofaq</t>
-  </si>
-  <si>
-    <t>Sort the array and use binary search like algorithm with two pointers</t>
-  </si>
-  <si>
-    <t>Use binary search like algorithm with two pointer technique.</t>
   </si>
 </sst>
 </file>
@@ -587,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,7 +592,7 @@
     <col min="1" max="1" width="8.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="31.88671875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="32.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="84.5546875" style="3" customWidth="1"/>
@@ -818,7 +812,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>53</v>
@@ -827,10 +821,10 @@
         <v>35</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -923,29 +917,6 @@
       </c>
       <c r="G14" s="6" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
-        <v>15</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -966,9 +937,8 @@
     <hyperlink ref="D5" r:id="rId11" xr:uid="{E51C5646-FEE1-44F7-91C4-364A6DFCFF85}"/>
     <hyperlink ref="D12" r:id="rId12" xr:uid="{EA1E0AA8-8F6F-4265-84F0-6C4AB0FA52AB}"/>
     <hyperlink ref="D10" r:id="rId13" xr:uid="{1D16F9F4-D9DC-49D7-A64B-F7F293ADC1B4}"/>
-    <hyperlink ref="D15" r:id="rId14" xr:uid="{D7A5DBEB-5A7C-4F40-9CC8-94EBF5CA0D24}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
longest repeating character replacement
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agneshk\pc\code\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F086D8-63B6-41A2-B0FF-99D02899FDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876810E7-2097-44A5-B053-EDE85AF8A18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="146">
   <si>
     <t>url</t>
   </si>
@@ -457,6 +457,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/longest-consecutive-sequence/description/</t>
+  </si>
+  <si>
+    <t>Using sliding window technique, check if (cur_len - len_max_repeats) &lt;= k.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-repeating-character-replacement/description/</t>
   </si>
 </sst>
 </file>
@@ -884,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -902,7 +908,7 @@
     <col min="8" max="8" width="8.88671875" style="1"/>
     <col min="9" max="9" width="8.88671875" style="5"/>
     <col min="10" max="10" width="29.21875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="73.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="80.88671875" style="1" customWidth="1"/>
     <col min="12" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
@@ -1877,59 +1883,39 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C35" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C36" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C37" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C38" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C39" s="3" t="s">
+    <row r="35" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="14">
+        <v>424</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="D35" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="F35" s="19">
+        <v>45510</v>
+      </c>
+      <c r="G35" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>99</v>
+      <c r="H35" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="I35" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J35" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="K35" s="16" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -1962,6 +1948,50 @@
         <v>120</v>
       </c>
       <c r="H42" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C43" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C44" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C45" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C46" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2002,8 +2032,9 @@
     <hyperlink ref="K31" r:id="rId29" xr:uid="{75FAD807-8F2F-4605-AA42-7430E89F39B4}"/>
     <hyperlink ref="K34" r:id="rId30" xr:uid="{DDD204B7-56F6-46D6-B0CA-16C89391A38C}"/>
     <hyperlink ref="K33" r:id="rId31" xr:uid="{9E4AB776-D33D-4E45-8AB2-CD1CF5D0EBBE}"/>
+    <hyperlink ref="K35" r:id="rId32" xr:uid="{0F61D851-BD73-4FFA-BA90-A9FD6037D508}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId32"/>
+  <pageSetup orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>